<commit_message>
Added Q4 FY25 and Q1 FY26 quarters for MRVL
</commit_message>
<xml_diff>
--- a/data/MRVL.xlsx
+++ b/data/MRVL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tngam\projects\python\stock-kpi-plot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tngam\projects\python\stock-kpi-plot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73A5E2D-6C6A-4C1C-9184-F3BEBC6161DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D946BAC8-9C88-4914-AD79-C98AC09967C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7290" yWindow="2360" windowWidth="28800" windowHeight="15370" xr2:uid="{847D2414-6927-4BEE-9896-7F31C50B6E3E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38380" windowHeight="20880" xr2:uid="{847D2414-6927-4BEE-9896-7F31C50B6E3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Report Date</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>Automotive/industrial</t>
+  </si>
+  <si>
+    <t>Q4 '25</t>
+  </si>
+  <si>
+    <t>Q1 '26</t>
   </si>
 </sst>
 </file>
@@ -104,10 +110,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -443,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7699876-666C-41D6-B24A-347A2FC5C849}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -458,7 +463,7 @@
     <col min="9" max="9" width="9.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -471,8 +476,14 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -487,76 +498,104 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>816.4</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>880.9</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>1101.0999999999999</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="2">
+        <v>1365.8</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1440.6</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>153.1</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>151</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>150.9</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2">
+        <v>171.4</v>
+      </c>
+      <c r="F4" s="2">
+        <v>177.5</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>71.8</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>75.900000000000006</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>84.7</v>
       </c>
+      <c r="E5" s="2">
+        <v>105.8</v>
+      </c>
+      <c r="F5" s="2">
+        <v>138.4</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>42</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>88.9</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>96.5</v>
       </c>
+      <c r="E6" s="2">
+        <v>88.7</v>
+      </c>
+      <c r="F6" s="2">
+        <v>63.1</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>77.599999999999994</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>76.2</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>82.9</v>
+      </c>
+      <c r="E7" s="2">
+        <v>85.7</v>
+      </c>
+      <c r="F7" s="2">
+        <v>75.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>